<commit_message>
updated files with most recent trained model
</commit_message>
<xml_diff>
--- a/model_comp.xlsx
+++ b/model_comp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cyntiakamogawa/Desktop/weather_prediction_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7755F8C7-AC6B-FE44-8301-FFA28705D33B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F01179-9030-9048-B623-2A8F8253A150}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4120" yWindow="2200" windowWidth="24640" windowHeight="10960" xr2:uid="{0047C147-AF68-A145-BEC5-AD6EB6711178}"/>
+    <workbookView xWindow="1260" yWindow="4820" windowWidth="24640" windowHeight="10960" xr2:uid="{0047C147-AF68-A145-BEC5-AD6EB6711178}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Manly</t>
   </si>
@@ -62,10 +62,13 @@
     <t>DTM final</t>
   </si>
   <si>
-    <t>RFR Final</t>
-  </si>
-  <si>
-    <t>KNR Final</t>
+    <t>1st</t>
+  </si>
+  <si>
+    <t>2nd</t>
+  </si>
+  <si>
+    <t>3rd</t>
   </si>
 </sst>
 </file>
@@ -93,7 +96,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -103,6 +106,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -119,13 +134,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,10 +465,13 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="6" max="6" width="10.83203125" style="12"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18">
       <c r="A1" s="2"/>
@@ -460,11 +485,9 @@
       <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="11"/>
+      <c r="G1" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18">
@@ -483,11 +506,9 @@
       <c r="E2" s="1">
         <v>0.312</v>
       </c>
-      <c r="F2" s="1">
-        <v>-117.38</v>
-      </c>
-      <c r="G2" s="1">
-        <v>-91.322000000000003</v>
+      <c r="F2" s="4"/>
+      <c r="G2" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18">
@@ -506,11 +527,9 @@
       <c r="E3" s="1">
         <v>-0.28799999999999998</v>
       </c>
-      <c r="F3" s="1">
-        <v>-32.332000000000001</v>
-      </c>
-      <c r="G3" s="1">
-        <v>-8.9269999999999996</v>
+      <c r="F3" s="4"/>
+      <c r="G3" s="10" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18">
@@ -520,7 +539,7 @@
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="6">
         <v>-0.11799999999999999</v>
       </c>
       <c r="D4" s="1">
@@ -529,12 +548,7 @@
       <c r="E4" s="5">
         <v>0.16300000000000001</v>
       </c>
-      <c r="F4" s="1">
-        <v>-322</v>
-      </c>
-      <c r="G4" s="1">
-        <v>-250.17</v>
-      </c>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:7" ht="18">
       <c r="A5" s="3">
@@ -543,7 +557,7 @@
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="6">
         <v>-0.79500000000000004</v>
       </c>
       <c r="D5" s="1">
@@ -552,12 +566,7 @@
       <c r="E5" s="1">
         <v>-1.966</v>
       </c>
-      <c r="F5" s="1">
-        <v>-5.4130000000000003</v>
-      </c>
-      <c r="G5" s="5">
-        <v>-0.34799999999999998</v>
-      </c>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:7" ht="18">
       <c r="A6" s="3">
@@ -566,21 +575,16 @@
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="7">
         <v>-3.3769999999999998</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="6">
         <v>-1.72</v>
       </c>
       <c r="E6" s="5">
         <v>-0.68799999999999994</v>
       </c>
-      <c r="F6" s="1">
-        <v>-162.69999999999999</v>
-      </c>
-      <c r="G6" s="1">
-        <v>-108.05</v>
-      </c>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:7" ht="18">
       <c r="A7" s="3">
@@ -589,7 +593,7 @@
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="6">
         <v>0.31490000000000001</v>
       </c>
       <c r="D7" s="5">
@@ -598,12 +602,7 @@
       <c r="E7" s="4">
         <v>0.26600000000000001</v>
       </c>
-      <c r="F7" s="1">
-        <v>-0.48499999999999999</v>
-      </c>
-      <c r="G7" s="1">
-        <v>-5.2999999999999999E-2</v>
-      </c>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:7" ht="18">
       <c r="A8" s="3">
@@ -612,21 +611,16 @@
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="7">
         <v>-3.1829999999999998</v>
       </c>
       <c r="D8" s="5">
         <v>-2.923</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="7">
         <v>-2.9910000000000001</v>
       </c>
-      <c r="F8" s="1">
-        <v>-5418.7</v>
-      </c>
-      <c r="G8" s="1">
-        <v>-4299.3999999999996</v>
-      </c>
+      <c r="F8" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
created tables and plots to analysis page
</commit_message>
<xml_diff>
--- a/model_comp.xlsx
+++ b/model_comp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cyntiakamogawa/Desktop/weather_prediction_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F01179-9030-9048-B623-2A8F8253A150}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE18ED14-52B3-0A46-9F20-C0DCA78547F5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="4820" windowWidth="24640" windowHeight="10960" xr2:uid="{0047C147-AF68-A145-BEC5-AD6EB6711178}"/>
+    <workbookView xWindow="-180" yWindow="860" windowWidth="24640" windowHeight="10960" xr2:uid="{0047C147-AF68-A145-BEC5-AD6EB6711178}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>Manly</t>
   </si>
@@ -75,7 +75,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -92,6 +92,11 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
@@ -134,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -142,12 +147,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,15 +470,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D9535A-F18C-994C-80FE-71411DAB508F}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="6" max="6" width="10.83203125" style="12"/>
+    <col min="6" max="6" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18">
@@ -485,8 +493,8 @@
       <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="8" t="s">
+      <c r="F1" s="10"/>
+      <c r="G1" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -497,17 +505,17 @@
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="12">
         <v>0.438</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>0.16400000000000001</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
         <v>0.312</v>
       </c>
       <c r="F2" s="4"/>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>11</v>
       </c>
     </row>
@@ -518,17 +526,17 @@
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="12">
         <v>-0.246</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>-0.56799999999999995</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <v>-0.28799999999999998</v>
       </c>
       <c r="F3" s="4"/>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>12</v>
       </c>
     </row>
@@ -539,13 +547,13 @@
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="13">
         <v>-0.11799999999999999</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>0.13800000000000001</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="12">
         <v>0.16300000000000001</v>
       </c>
       <c r="F4" s="4"/>
@@ -557,13 +565,13 @@
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="13">
         <v>-0.79500000000000004</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>-1.2789999999999999</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="2">
         <v>-1.966</v>
       </c>
       <c r="F5" s="4"/>
@@ -575,13 +583,13 @@
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="14">
         <v>-3.3769999999999998</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="13">
         <v>-1.72</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="12">
         <v>-0.68799999999999994</v>
       </c>
       <c r="F6" s="4"/>
@@ -593,13 +601,13 @@
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="13">
         <v>0.31490000000000001</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="12">
         <v>0.39700000000000002</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="10">
         <v>0.26600000000000001</v>
       </c>
       <c r="F7" s="4"/>
@@ -611,16 +619,135 @@
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="14">
         <v>-3.1829999999999998</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="12">
         <v>-2.923</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="13">
         <v>-2.9910000000000001</v>
       </c>
       <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" ht="18">
+      <c r="A9" s="3">
+        <v>43496</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.35699999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18">
+      <c r="A10" s="3">
+        <v>43496</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5">
+        <v>-0.16600000000000001</v>
+      </c>
+      <c r="D10" s="6">
+        <v>-0.193</v>
+      </c>
+      <c r="E10" s="1">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="18">
+      <c r="A11" s="3">
+        <v>43496</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="15">
+        <v>0.128</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="E11" s="1">
+        <v>5.1999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18">
+      <c r="A12" s="3">
+        <v>43496</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="5">
+        <v>-0.90200000000000002</v>
+      </c>
+      <c r="D12" s="6">
+        <v>-1.3620000000000001</v>
+      </c>
+      <c r="E12" s="1">
+        <v>-1.899</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18">
+      <c r="A13" s="3">
+        <v>43496</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1">
+        <v>-1.758</v>
+      </c>
+      <c r="D13" s="5">
+        <v>-0.63500000000000001</v>
+      </c>
+      <c r="E13" s="6">
+        <v>-6.7000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18">
+      <c r="A14" s="3">
+        <v>43496</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0.27600000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18">
+      <c r="A15" s="3">
+        <v>43496</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="6">
+        <v>-1.3879999999999999</v>
+      </c>
+      <c r="D15" s="5">
+        <v>-1.069</v>
+      </c>
+      <c r="E15" s="1">
+        <v>-1.8380000000000001</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>